<commit_message>
try to update files
</commit_message>
<xml_diff>
--- a/Indeed/data_result/Python Developer.xlsx
+++ b/Indeed/data_result/Python Developer.xlsx
@@ -453,63 +453,63 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Application Developer</t>
+          <t>Backend Developer</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bank Mega</t>
+          <t>Ensoft</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Bank-Mega</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>HRIS Developer</t>
+          <t>Senior Software Developer</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Binabusana Internusa</t>
+          <t>Oracle</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Oracle</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Java Developer</t>
+          <t>Software Quality Assurance Intern</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NTT Ltd</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Game Developer</t>
+          <t>Data Scientist</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alegrium</t>
+          <t>Lancar</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -521,12 +521,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Lead Instructors - Le Wagon Data Science Bootcamp</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1rstWAP</t>
+          <t>Le Wagon Bali</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -538,12 +538,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT Production Support (Jakarta) - remote</t>
+          <t>ERP Consultant / ERP Implementator</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lennor Metier Consulting Philippines</t>
+          <t>HashMicro</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -555,12 +555,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Python Programmer</t>
+          <t>DevOps Engineer (Work from Home; Full-time)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>1rstWAP</t>
+          <t>Dynamic Technology Lab Pte Ltd</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -572,12 +572,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>HRIS Developer</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IndoSterling Technomedia</t>
+          <t>Binabusana Internusa</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -589,12 +589,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IT DATA ENGINEER</t>
+          <t>Head of Data</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PT. Kwadran Lima Mitra Kaya Solusi</t>
+          <t>PT Sinar Mas Digital Ventures</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -606,12 +606,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>(Singapore Corp) Python Software Developer</t>
+          <t>Python Programmer</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MatchaTalent</t>
+          <t>1rstWAP</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -623,29 +623,29 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IT WEB DEVELOPER</t>
+          <t>Publisher Support Specialist</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ismaya Group</t>
+          <t>Coda Payments</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Ismaya-Group-1</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Senior Back End Developer</t>
+          <t>Business Intelligence Developer E-Commerce</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Sonar Social Media Monitoring Platform</t>
+          <t>Kompas Gramedia</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -657,46 +657,46 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Full-Stack Developer</t>
+          <t>ShopeePay QA Engineer [Entry Level] - NEW</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DDTC</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BACKEND DEVELOPER</t>
+          <t>ShopeePay Backend Engineer [Experienced]</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Dipstrategy</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C# Software Developer, Trilogy (Remote) - $100,000/year USD</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Crossover</t>
+          <t>1rstWAP</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -708,12 +708,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ERP Consultant / ERP Implementator</t>
+          <t>ERP Developer</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>HashMicro</t>
+          <t>PT Monotaro Indonesia</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -725,12 +725,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Python Developer</t>
+          <t>Senior Backend Developer</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>QSI Recruitment</t>
+          <t>AiChat Pte Ltd</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -742,12 +742,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Great Giant Foods</t>
+          <t>Renos.id</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -759,12 +759,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Full Stack Developer</t>
+          <t>PHP Developer</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ensoft</t>
+          <t>PT Media Mitrakarya Indonesia</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -776,12 +776,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Unity Developer</t>
+          <t>System Administrator</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Alegrium</t>
+          <t>Jawasoft</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -793,12 +793,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Web Developer</t>
+          <t>Full Stack/Backend Developer</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Binabusana Internusa</t>
+          <t>TPG Telecom Pte Ltd</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -810,12 +810,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Senior Backend Developer</t>
+          <t>Fullstack Developer</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>DETIKcom</t>
+          <t>PT Hermes Solusi Integrasi</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -827,12 +827,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Business Intelligence Developer</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Stockbit-Bibit</t>
+          <t>PopBox</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -844,12 +844,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Senior Frontend Developer</t>
+          <t>IT Production Support (Remote)</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ensoft</t>
+          <t>mClinica</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -861,12 +861,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Pintek ID</t>
+          <t>Ensoft</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -878,46 +878,46 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Senior Developer - Network (contract based)</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Standard Chartered</t>
+          <t>Great Giant Foods</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Standard-Chartered-Bank</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Business Intelligence Developer E-Commerce</t>
+          <t>Software Quality Assurance - Manual Testing</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Kompas Gramedia</t>
+          <t>Cermati.com</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Kompas-Gramedia-Group</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>IT Developer</t>
+          <t>ODOO developer/Junior&amp;Senior Developer/Software engineer.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MNC</t>
+          <t>PT. Virgo Stellar</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -929,29 +929,29 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>System Administrator</t>
+          <t>Application Developer</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jawasoft</t>
+          <t>Bank Mega</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Bank-Mega</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Senior Software Developer, Trilogy (Remote) - $100,000/year...</t>
+          <t>Golang Developer</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Crossover</t>
+          <t>PT. Indocyber Global Technology</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -963,29 +963,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>IT Engineer</t>
+          <t>Developer / Programmer</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PT Bank Central Asia Tbk</t>
+          <t>StrategArt</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/PT-Bank-Central-Asia-Tbk</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Product Support Engineer</t>
+          <t>Web Developer</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>JULO</t>
+          <t>Binabusana Internusa</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -997,12 +997,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>Lead Software Quality Assurance</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Haswara Anjaya Akeh (Haswara Anjaya Akeh) PT</t>
+          <t>Cermati.com</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1014,12 +1014,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Senior Backend Developer</t>
+          <t>Back End Developer</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Schoters</t>
+          <t>Akseleran</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1031,12 +1031,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Test Engineer</t>
+          <t>Developer</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Quipper</t>
+          <t>Kinarya Alihdaya Mandiri PT</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1048,29 +1048,29 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Senior Machine Learning</t>
+          <t>Senior Developer - Network (contract based)</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Alodokter</t>
+          <t>Standard Chartered</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Alodokter-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>Technical Operations Engineer</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tokenomy</t>
+          <t>byOrange</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1082,143 +1082,143 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Data Warehouse Engineer</t>
+          <t>Golang Developer (Back End)</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>PT Lunaria Annua Teknologi (KoinWorks)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Senior Engineering Manager II Remote</t>
+          <t>Datawarehouse Data Analyst (working in Kuala Lumpur, Malaysi...</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Kalibrr</t>
+          <t>Mission Consultancy Services Malaysia SDN BHD</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Kalibrr-Teknologi-Personalia</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Software Engineer, xShop</t>
+          <t>Front End Development – Consultant</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Coda Payments</t>
+          <t>Accenture</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Accenture</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Machine Learning Engineer</t>
+          <t>QA Engineer</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Nomura Research Institute Indonesia</t>
+          <t>StyleTheory</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Styletheory</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Golang Developer (Back End)</t>
+          <t>IBM Service Associate Program - Application Developer</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>PT Lunaria Annua Teknologi (KoinWorks)</t>
+          <t>IBM</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/IBM</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ShopeePay QA Engineer [Entry Level] - NEW</t>
+          <t>Backend Engineer</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>Cicil</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Back End Developer</t>
+          <t>IT WEB DEVELOPER</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>PT Generasi Teknologi Buana</t>
+          <t>Ismaya Group</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Ismaya-Group-1</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Engineering and Technology - Back End Engineer, Payment Proc...</t>
+          <t>Associate Backend Engineer</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>KeDA Tech</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Data Warehouse Engineer - GoPay</t>
+          <t>Data Warehouse Engineer</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1235,63 +1235,63 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Consultant - Intelligent Automation - ID</t>
+          <t>Data Warehouse Engineer - GoPay</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Deloitte</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Deloitte</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ERP Developer</t>
+          <t>ShopeePay QA Engineer [Experienced]</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>PT Monotaro Indonesia</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Fullstack Developer - Javascript, Python, Golang, NodeJS, Re...</t>
+          <t>Java Developer</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Michael Page</t>
+          <t>NTT Ltd</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Michael-Page</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Technical Operations Engineer</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>byOrange</t>
+          <t>Vicuna Corp</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1303,12 +1303,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SDET (Automation Engineer)</t>
+          <t>Senior Developer</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>FinAccel</t>
+          <t>PT Chrombit Digtal Lab</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1320,12 +1320,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Data Engineer (ETL Developer)</t>
+          <t>System Engineering Development</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Lawencon International PT</t>
+          <t>Alodokter</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1337,29 +1337,29 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Back end developer</t>
+          <t>Financial Service SRE Engineer [Entry Level]</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>MNC</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Test Engineer</t>
+          <t>Business Intelligence Developer</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>LINE Plus corporation</t>
+          <t>Stockbit-Bibit</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1371,46 +1371,46 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Engineering and Technology - System Quality Assurance</t>
+          <t>ERP Programmer (Odoo Framework)</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>HashMicro</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Technical Consultant Assc.</t>
+          <t>Python Developer</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Mitra Integrasi Informatika</t>
+          <t>QSI Recruitment</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Mitra-Integrasi-Informatika</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Associate Backend Engineer</t>
+          <t>Software Engineer - Data Platform</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>KeDA Tech</t>
+          <t>Cermati.com</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1422,29 +1422,29 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Senior Data Warehouse Engineer - GoPay</t>
+          <t>Senior Backend Developer</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>Schoters</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Engineer: Software Developer</t>
+          <t>Senior Machine Learning</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>NTT Ltd</t>
+          <t>Alodokter</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1456,46 +1456,46 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Data Engineer</t>
+          <t>Integration Developer</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Pintap</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Senior Data Warehouse Engineer</t>
+          <t>Customer Solutions Consultant, Infrastructure Modernization,...</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>Google</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>https://id.indeed.com//cmp/Google</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Remote) QA Engineer SDET</t>
+          <t>Software Engineer, xShop</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Kitabisa.com</t>
+          <t>Coda Payments</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1507,63 +1507,63 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>ShopeePay QA Engineer [Experienced]</t>
+          <t>QA Engineer - GoFinance</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>GO-JEK</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>ERP Programmer (Odoo Framework)</t>
+          <t>ShopeePay Backend Engineer [Leader]</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>HashMicro</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>ShopeePay Backend Engineer [Experienced]</t>
+          <t>API Developer</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Shopee</t>
+          <t>PT Multi Bangun Abadi</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Shopee</t>
+          <t>https://id.indeed.com//cmp/PT-Multi-Bangun-Abadi</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Sales Engineer</t>
+          <t>Software Engineer</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Dynatrace</t>
+          <t>Alterra</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -1575,12 +1575,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Software Engineer</t>
+          <t>Data Engineer</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Alterra</t>
+          <t>Tokenomy</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -1592,63 +1592,63 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>System Engineering Development</t>
+          <t>BACKEND DEVELOPER</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Alodokter</t>
+          <t>Dipstrategy</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Alodokter-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Database Development Engineer</t>
+          <t>Engineering and Technology - Sea Labs - Back End Engineer, P...</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ATS Global</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Link is not available</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Finance MIS Analyst - Financial Services</t>
+          <t>Senior Back End Developer</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>GO-JEK</t>
+          <t>Sonar Social Media Monitoring Platform</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Pt.-Go--jek-Indonesia-2</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Backend Developer</t>
+          <t>Test Engineer</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>PT Quantum Select International</t>
+          <t>Quipper</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1660,17 +1660,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Solutions Architect - Developer Specialist</t>
+          <t>Productivity Engineer</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>PT Amazon Web Services IDN</t>
+          <t>Stockbit-Bibit</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/Amazon.com</t>
+          <t>Link is not available</t>
         </is>
       </c>
     </row>
@@ -1694,29 +1694,29 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IBM Service Associate Program - Application Developer</t>
+          <t>Engineering and Technology - Sea Labs - System Quality Assur...</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>IBM</t>
+          <t>Shopee</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://id.indeed.com//cmp/IBM</t>
+          <t>https://id.indeed.com//cmp/Shopee</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>ETL Developer</t>
+          <t>QA Automation Engineer</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Lawencon</t>
+          <t>Nimbly</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">

</xml_diff>